<commit_message>
first face-to-face discussion of MHDS comments
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-First.xlsx
+++ b/MHDS/MHDS-Comment-First.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541D76E5-22F6-443C-A68B-F385E5EC8685}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435DCA0C-F169-4B97-A2AF-EE6B0389B525}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="247">
   <si>
     <t>Priority</t>
   </si>
@@ -723,12 +723,284 @@
   <si>
     <t>Systems Design choice. Not IHE scope. It is possible, but then isn't that just MHD+XDS as is already documented by MHD?</t>
   </si>
+  <si>
+    <t>make clear in MHDS that this is a pre-condition to registry</t>
+  </si>
+  <si>
+    <t>mCSD supports consistent coding and cross referencing between provider, organization, location and service IDs</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">expand to reference all capabilities of mCSD (not CSDm)… and indicate that the MHDS solution is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF666666"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>also</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF666666"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> leveraged to enforce the consistent use of a reference set of managed enterprise IDs for locations, organizations and servivces.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Open issue 3.a seems to suggest that this is a MAY rather than a SHALL. It should be a SHALL that the MHDS registry would reject with an exception any inbound content that did NOT reference a valid (managed) provider ID, location ID, organization ID or service ID. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">propose this be strengthened… the overall HIE won't worlk, otherwise. Although there isn't much focus on location registry in the US or Canada (for example) this is a really important requirement in LMIC settings. </t>
+  </si>
+  <si>
+    <t>agree that open issue 4.a should be addressed as a mandatory reference to an enterprise patient ID (golden record reference)</t>
+  </si>
+  <si>
+    <t>as with above… it seems there is no downside to making mandatory the reference to a golden patient ID and it seems like it will simplify things quite a bit.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">it isn't clear in the descripiont of Open issue 5 whether a Document Repository actor is a necessary pre-condition for "on demand documents" (ODD) functionality to be supported. The need for ODD is very high -- especially in LMICs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in any of the use cases related to IPS being leveraged by CCG content profiles. IF a Document Repository actor is needed for ODD... then a Document Repository actor is likely needed to MHDS. NOTE... the analogous ODD support in XDS requires an ODD Source </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a Document Repository </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>an Integrated Document Source/Repository... so maybe we should look for a FHIR-based ODD Source as our option in MHDS.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IF a Doc Repo actor is needed for MHDS to support ODD… THEN a Doc Repo actor should be included… this is an important use case. </t>
+  </si>
+  <si>
+    <t>278, 300, 357</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">expand to reference all capabilities of mCSD (not CSDm)… and indicate that the MHDS solution may be also leveraged to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>enforce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> the consistent use of a reference set of managed enterprise IDs</t>
+    </r>
+  </si>
+  <si>
+    <t>recommend mCSD as a required grouping and mandatory checking of inbound documents against the provider, location, organization (where applicable) and service (maybe overlaps with SVCM)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">make mCSD grouping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">mandataory </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>for MHDS</t>
+    </r>
+  </si>
+  <si>
+    <t>There is a pretty high likelihood that MHDS will need to operate in a message + document setting where some (but not all) of the content is conveyed by FHIR documents. What is the expected behaviour of the HIE under these circumstances?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Define an expected behaviour when there is both information about a subject of care that has been conveyed to the FHIR server as FHIR documents </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> there is information that has been conveyed as FHIR messages. What should a requestor do to get ALL the relevant information? And how might this impact ODD (or does ODD maybe solve this issue)? Basically... should a requestor expect to get the same set of clinical content if they asked for EVERYTHING via ITI-68 (embedded inside the resulting documents, of course... and they could pull it out using mXDE) as they would get if they asked for EVERYTHING via PCC-44? [NOTE closed issue mXDE_202 discusses this situation and it is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>not resolved</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>...]</t>
+    </r>
+  </si>
+  <si>
+    <t>Derek Ritz</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>decided to fully support this option, which means adding an option on MHD for non-contained</t>
+  </si>
+  <si>
+    <t>agreed under the option this would be the case</t>
+  </si>
+  <si>
+    <t>on-demand and defered-assembly are out-of-scope at this time. They would come in a future work item. They are not related to the repository issue… Note that a purely FHIR function like on-demand and defered-assmbly exist and are very different than XDS.</t>
+  </si>
+  <si>
+    <t>check location</t>
+  </si>
+  <si>
+    <t>messages that are persisted are a legitimate type of 'document'. The definition of 'document' in XDS and MHD are broad. They are not restricted to the definition of Document found in CDA.
+Not clear what action is being asked regarding mXDE.</t>
+  </si>
+  <si>
+    <t>Need to mention early that client sides are explicitly normal MHD clients with no additional requirements. This is only said much later in the intergration statement section</t>
+  </si>
+  <si>
+    <t>agreed. Some form of diagrams similar to provided would be useful.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to the same extent as in normal MHD. </t>
+  </si>
+  <si>
+    <t>agreed to move this to X.7, and invent an X.4 that is more classic use-case driven. This new X.4 can leverage the X.7 text.</t>
+  </si>
+  <si>
+    <t>Decided: We will add a "repository" option to the Registry to indicate a registry that supports persisting binary, and the absence of the option would reject transactions including a binary. Also agreed to add a Repository Actor, so that there is something to point at in overall diagrams and associate attachment.url with. We agreed to NOT create inline transactions on the publication side involving the repository so that we don't need to break from MHD.</t>
+  </si>
+  <si>
+    <t>see #23</t>
+  </si>
+  <si>
+    <t>review as I thought I was clear that although it is designed to be implementable with one centeral system, it can be implemented with purpose specific systems</t>
+  </si>
+  <si>
+    <t>NO. If XDS is involed them use MHD. MHDS is for environments that do NOT have XDS
+POSSIBLE: Is this a request to support XDS Document Source publishing to an MHDS backend? That would also be a new-work-item, but not one proposed so far.</t>
+  </si>
+  <si>
+    <t>done?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,13 +1032,55 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -876,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -925,6 +1239,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1264,13 +1590,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,10 +1606,11 @@
     <col min="3" max="3" width="10.28515625" style="14" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="14" customWidth="1"/>
     <col min="5" max="5" width="60.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="67.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="54.140625" style="14" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="14" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="14"/>
+    <col min="9" max="9" width="26.28515625" style="14" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1315,7 +1642,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1388,7 +1715,9 @@
       <c r="H4" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1415,7 +1744,9 @@
       <c r="H5" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1492,7 +1823,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>64</v>
       </c>
@@ -1515,9 +1846,11 @@
       <c r="H9" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>64</v>
       </c>
@@ -1540,7 +1873,9 @@
       <c r="H10" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="7" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1587,7 +1922,7 @@
       <c r="G12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="17" t="s">
         <v>199</v>
       </c>
       <c r="I12" s="7"/>
@@ -1641,7 +1976,7 @@
       <c r="G14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="17" t="s">
         <v>200</v>
       </c>
       <c r="I14" s="7"/>
@@ -1777,7 +2112,9 @@
       <c r="H19" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="7" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1850,7 +2187,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="154.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>106</v>
       </c>
@@ -1873,9 +2210,11 @@
       <c r="H23" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="13" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>110</v>
       </c>
@@ -1899,6 +2238,9 @@
       </c>
       <c r="H24" s="14" t="s">
         <v>207</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="180" x14ac:dyDescent="0.25">
@@ -1920,6 +2262,9 @@
       <c r="H25" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="I25" s="14" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -1960,8 +2305,11 @@
       <c r="H27" s="14" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="I27" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>113</v>
       </c>
@@ -1979,8 +2327,14 @@
       <c r="G28" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="H28" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>113</v>
       </c>
@@ -1996,6 +2350,12 @@
       <c r="G29" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="H29" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
@@ -2017,6 +2377,9 @@
       </c>
       <c r="H30" s="14" t="s">
         <v>209</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
@@ -2040,6 +2403,9 @@
       <c r="H31" s="14" t="s">
         <v>210</v>
       </c>
+      <c r="I31" s="14" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
@@ -2062,8 +2428,11 @@
       <c r="H32" s="14" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I32" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>122</v>
       </c>
@@ -2085,7 +2454,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>122</v>
       </c>
@@ -2107,7 +2476,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>122</v>
       </c>
@@ -2129,7 +2498,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>140</v>
       </c>
@@ -2150,8 +2519,11 @@
       <c r="H36" s="14" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I36" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>140</v>
       </c>
@@ -2175,7 +2547,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>140</v>
       </c>
@@ -2195,7 +2567,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>150</v>
       </c>
@@ -2219,7 +2591,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>150</v>
       </c>
@@ -2240,10 +2612,10 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>150</v>
       </c>
@@ -2267,7 +2639,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>162</v>
       </c>
@@ -2291,7 +2663,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>162</v>
       </c>
@@ -2314,8 +2686,11 @@
       <c r="H43" s="14" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I43" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>162</v>
       </c>
@@ -2339,7 +2714,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>162</v>
       </c>
@@ -2363,7 +2738,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>162</v>
       </c>
@@ -2387,7 +2762,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>162</v>
       </c>
@@ -2408,8 +2783,11 @@
       <c r="H47" s="14" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="I47" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>184</v>
       </c>
@@ -2426,10 +2804,13 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>184</v>
       </c>
@@ -2446,8 +2827,11 @@
       <c r="H49" s="14" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="I49" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>184</v>
       </c>
@@ -2463,6 +2847,156 @@
       <c r="G50" s="16"/>
       <c r="H50" s="14" t="s">
         <v>215</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" s="19">
+        <v>149</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="18">
+        <v>174</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="18">
+        <v>180</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="18">
+        <v>184</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="18">
+        <v>439</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D57" s="18">
+        <v>593</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="G57" s="18"/>
+      <c r="H57" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revisions from today face-to-face
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-First.xlsx
+++ b/MHDS/MHDS-Comment-First.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C68157E-69B8-4E97-A1FE-59EAAFED0C9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE39398-E175-43B4-9FCC-DB22777CEA2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="260">
   <si>
     <t>Priority</t>
   </si>
@@ -664,16 +664,7 @@
     <t>yes</t>
   </si>
   <si>
-    <t>possibly. Need the IUA team to help</t>
-  </si>
-  <si>
     <t xml:space="preserve">I don't think there is a centeral source of identity. </t>
-  </si>
-  <si>
-    <t>this does seem to becoming true. There is drive to have more relaxed metadata than XDS or minimal</t>
-  </si>
-  <si>
-    <t>yes? Good time to discuss this plan. What is not clear is what is always 'or better'</t>
   </si>
   <si>
     <t>BPPC and to some extent APPC would work. But we likely need to write a FHIR Consent profile to better fit the needs of MHDS</t>
@@ -974,9 +965,6 @@
     <t>agreed. Some form of diagrams similar to provided would be useful.</t>
   </si>
   <si>
-    <t xml:space="preserve">to the same extent as in normal MHD. </t>
-  </si>
-  <si>
     <t>agreed to move this to X.7, and invent an X.4 that is more classic use-case driven. This new X.4 can leverage the X.7 text.</t>
   </si>
   <si>
@@ -984,16 +972,10 @@
   </si>
   <si>
     <t>see #23</t>
-  </si>
-  <si>
-    <t>review as I thought I was clear that although it is designed to be implementable with one centeral system, it can be implemented with purpose specific systems</t>
   </si>
   <si>
     <t>NO. If XDS is involed them use MHD. MHDS is for environments that do NOT have XDS
 POSSIBLE: Is this a request to support XDS Document Source publishing to an MHDS backend? That would also be a new-work-item, but not one proposed so far.</t>
-  </si>
-  <si>
-    <t>done?</t>
   </si>
   <si>
     <t>Yes, require FHIR audit logging</t>
@@ -1007,6 +989,54 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>no. the Registry is grouped with IUA Resource Server to do enforcement, but the IUA Resource Client is part of the client system on the Document Consumer</t>
+  </si>
+  <si>
+    <t>diagrams need updating</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>I think this is point out the client actors within the MHDS Document Registry (PIMR, SVCM, mCSD, and ATNA) might use IUA when calling out to the services in the infrastructure. This might be true, but it is not clear that we have a mandate in MHDS. Should we require it anyway? Service to service is not common to use IUA, but rather just use ATNA Secure Node.</t>
+  </si>
+  <si>
+    <t>I think this is point out the Patient Identity client actors within the MHDS Document Registry might use IUA when calling out to the services in the infrastructure. I have not used that model, I have followed the XDS model where the Document Registry receives the PIMR feed so that it is knowledgeable of all identity, thus it does not need to query PIMR in realtime.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes. </t>
+  </si>
+  <si>
+    <t>ITI</t>
+  </si>
+  <si>
+    <t>author reference option requires relaxing MHD requirements. Thus to include this option means we must update the MHD profile. Should we hold off on this option until we can do both?</t>
+  </si>
+  <si>
+    <t>Should MHDS require comprehensive metadata? If so, see author reference option. In the absence of a profiled requirement, this could be managed with error handling. That is that the Registry can fail publication requests that don't mee some configured metadata requirement. This was not the approach with XDS, so should it be the approach with MHD. The comprehensive metadata has proven to be useful in XDS as it requires more useful metadata, right? Or did we overly constrain the metadata under an expectation it would be better, when our requirements might be lighter now that we are more experienced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">informative text in section X.7 </t>
+  </si>
+  <si>
+    <t>no change</t>
+  </si>
+  <si>
+    <t>I think that all the content here is cross-profile considerations. It is not including any communication within the Document Registry</t>
+  </si>
+  <si>
+    <t>no the X.1-1 is including as one block the MHDS Document Registry. The X.1-2 is exploding out what the one block is in detail.</t>
+  </si>
+  <si>
+    <t>federation of MHDS is not in scope</t>
+  </si>
+  <si>
+    <t>added definitions for the persona in the flow</t>
+  </si>
+  <si>
+    <t>fixed different ways</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1112,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1203,7 +1239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1267,6 +1303,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1606,13 +1651,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1703,7 @@
         <v>192</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
@@ -1710,6 +1755,9 @@
         <v>195</v>
       </c>
       <c r="I3" s="7"/>
+      <c r="J3" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1735,7 +1783,10 @@
         <v>193</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
@@ -1764,7 +1815,7 @@
         <v>194</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1791,8 +1842,11 @@
         <v>195</v>
       </c>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="J6" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
@@ -1813,9 +1867,11 @@
         <v>8</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>244</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1838,11 +1894,16 @@
         <v>7</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="216.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>64</v>
       </c>
@@ -1862,14 +1923,12 @@
       <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="H9" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="216.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>64</v>
       </c>
@@ -1889,14 +1948,14 @@
       <c r="G10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>195</v>
+      <c r="H10" s="22" t="s">
+        <v>248</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>64</v>
       </c>
@@ -1917,11 +1976,11 @@
         <v>9</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>64</v>
       </c>
@@ -1942,10 +2001,13 @@
         <v>8</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1971,9 +2033,14 @@
         <v>8</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="I13" s="7"/>
+        <v>199</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="14" spans="1:10" s="4" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1998,13 +2065,13 @@
         <v>8</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -2030,11 +2097,11 @@
         <v>8</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="4" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
@@ -2060,11 +2127,14 @@
         <v>8</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>64</v>
       </c>
@@ -2090,8 +2160,11 @@
         <v>195</v>
       </c>
       <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="J17" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>64</v>
       </c>
@@ -2112,11 +2185,14 @@
         <v>8</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="J18" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>64</v>
       </c>
@@ -2139,13 +2215,16 @@
         <v>8</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
@@ -2166,11 +2245,16 @@
         <v>8</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" s="4" customFormat="1" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="115.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>64</v>
       </c>
@@ -2191,11 +2275,16 @@
         <v>8</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>104</v>
       </c>
@@ -2210,13 +2299,16 @@
         <v>7</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>106</v>
       </c>
@@ -2237,13 +2329,13 @@
         <v>8</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="I23" s="13" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>110</v>
       </c>
@@ -2266,13 +2358,16 @@
         <v>8</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>113</v>
       </c>
@@ -2289,13 +2384,16 @@
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>113</v>
       </c>
@@ -2312,8 +2410,11 @@
       <c r="H26" s="14" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J26" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -2332,13 +2433,13 @@
         <v>9</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>113</v>
       </c>
@@ -2357,13 +2458,16 @@
         <v>9</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>113</v>
       </c>
@@ -2380,13 +2484,16 @@
         <v>9</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>122</v>
       </c>
@@ -2405,13 +2512,16 @@
         <v>9</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>122</v>
       </c>
@@ -2430,13 +2540,16 @@
         <v>9</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>122</v>
       </c>
@@ -2455,13 +2568,13 @@
         <v>9</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>122</v>
       </c>
@@ -2480,10 +2593,16 @@
         <v>9</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>122</v>
       </c>
@@ -2502,10 +2621,16 @@
         <v>9</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>122</v>
       </c>
@@ -2524,10 +2649,16 @@
         <v>8</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>140</v>
       </c>
@@ -2546,13 +2677,13 @@
         <v>9</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>140</v>
       </c>
@@ -2573,10 +2704,16 @@
         <v>8</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>140</v>
       </c>
@@ -2593,10 +2730,16 @@
         <v>7</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>150</v>
       </c>
@@ -2617,10 +2760,13 @@
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>150</v>
       </c>
@@ -2641,10 +2787,16 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="14" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>150</v>
       </c>
@@ -2665,10 +2817,13 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>162</v>
       </c>
@@ -2689,10 +2844,13 @@
         <v>7</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>162</v>
       </c>
@@ -2713,13 +2871,16 @@
         <v>8</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>162</v>
       </c>
@@ -2740,10 +2901,13 @@
         <v>7</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>162</v>
       </c>
@@ -2764,10 +2928,13 @@
         <v>7</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>162</v>
       </c>
@@ -2788,10 +2955,16 @@
         <v>7</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>162</v>
       </c>
@@ -2810,13 +2983,13 @@
         <v>8</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>184</v>
       </c>
@@ -2833,13 +3006,16 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="14" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>184</v>
       </c>
@@ -2854,13 +3030,16 @@
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
       <c r="H49" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="J49" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>184</v>
       </c>
@@ -2875,157 +3054,185 @@
       <c r="F50" s="16"/>
       <c r="G50" s="16"/>
       <c r="H50" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="J50" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D51" s="18">
         <v>149</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F51" s="17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G51" s="18" t="s">
         <v>9</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D52" s="17">
         <v>174</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F52" s="17" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>9</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D53" s="17">
         <v>180</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>9</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D54" s="17">
         <v>184</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F55" s="17" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D56" s="17">
         <v>439</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F56" s="17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D57" s="17">
         <v>593</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F57" s="17" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>246</v>
+        <v>254</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates from Wednesday face-to-face
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-First.xlsx
+++ b/MHDS/MHDS-Comment-First.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE39398-E175-43B4-9FCC-DB22777CEA2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0445986-88BD-4396-B2FE-45ABA838B625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="265">
   <si>
     <t>Priority</t>
   </si>
@@ -962,13 +962,7 @@
     <t>Need to mention early that client sides are explicitly normal MHD clients with no additional requirements. This is only said much later in the intergration statement section</t>
   </si>
   <si>
-    <t>agreed. Some form of diagrams similar to provided would be useful.</t>
-  </si>
-  <si>
     <t>agreed to move this to X.7, and invent an X.4 that is more classic use-case driven. This new X.4 can leverage the X.7 text.</t>
-  </si>
-  <si>
-    <t>Decided: We will add a "repository" option to the Registry to indicate a registry that supports persisting binary, and the absence of the option would reject transactions including a binary. Also agreed to add a Repository Actor, so that there is something to point at in overall diagrams and associate attachment.url with. We agreed to NOT create inline transactions on the publication side involving the repository so that we don't need to break from MHD.</t>
   </si>
   <si>
     <t>see #23</t>
@@ -994,27 +988,18 @@
     <t>no. the Registry is grouped with IUA Resource Server to do enforcement, but the IUA Resource Client is part of the client system on the Document Consumer</t>
   </si>
   <si>
-    <t>diagrams need updating</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>I think this is point out the client actors within the MHDS Document Registry (PIMR, SVCM, mCSD, and ATNA) might use IUA when calling out to the services in the infrastructure. This might be true, but it is not clear that we have a mandate in MHDS. Should we require it anyway? Service to service is not common to use IUA, but rather just use ATNA Secure Node.</t>
   </si>
   <si>
-    <t>I think this is point out the Patient Identity client actors within the MHDS Document Registry might use IUA when calling out to the services in the infrastructure. I have not used that model, I have followed the XDS model where the Document Registry receives the PIMR feed so that it is knowledgeable of all identity, thus it does not need to query PIMR in realtime.</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes. </t>
   </si>
   <si>
     <t>ITI</t>
   </si>
   <si>
-    <t>author reference option requires relaxing MHD requirements. Thus to include this option means we must update the MHD profile. Should we hold off on this option until we can do both?</t>
-  </si>
-  <si>
     <t>Should MHDS require comprehensive metadata? If so, see author reference option. In the absence of a profiled requirement, this could be managed with error handling. That is that the Registry can fail publication requests that don't mee some configured metadata requirement. This was not the approach with XDS, so should it be the approach with MHD. The comprehensive metadata has proven to be useful in XDS as it requires more useful metadata, right? Or did we overly constrain the metadata under an expectation it would be better, when our requirements might be lighter now that we are more experienced?</t>
   </si>
   <si>
@@ -1037,6 +1022,36 @@
   </si>
   <si>
     <t>fixed different ways</t>
+  </si>
+  <si>
+    <t>These are internal conversations that are not part of IUA. So no change</t>
+  </si>
+  <si>
+    <t>no formal use beyond Registry protection of the MHD transactions. Beyond that is possible by the developer, it is just not defined by us. If we were to bring that in, then we would be bringing in the full set of services in the infrastructure.</t>
+  </si>
+  <si>
+    <t>PDQm is included under an option, but not otherwise.</t>
+  </si>
+  <si>
+    <t>add a discussion of organization requirements when they choose to host the binary elswhere</t>
+  </si>
+  <si>
+    <t>simply close the issue as this is already allowed by MHD… check that assertion</t>
+  </si>
+  <si>
+    <t>need to pick a scope pattern, and create an open issue asking for comment on the scope pattern we chose.</t>
+  </si>
+  <si>
+    <t>given that we are requiring Document Registry receive the PIMR feed, is there a good reason to keep the PIMR Query option? It would be useful to prevent duplication of data in the Document Registry, but it is such an obvious systems design decision that it may not need a specific option.</t>
+  </si>
+  <si>
+    <t>remove option</t>
+  </si>
+  <si>
+    <t>pick the last option with standalone PurposeOfUse and queryParam. Explain it neither relies on nor conflicts with SMART-on-FHIR scopes. Include two examples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lynn is improving them given current discussions. </t>
   </si>
 </sst>
 </file>
@@ -1651,13 +1666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J59"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1718,7 @@
         <v>192</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
@@ -1814,8 +1829,8 @@
       <c r="H5" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>236</v>
+      <c r="I5" s="22" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1867,10 +1882,13 @@
         <v>8</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>245</v>
+        <v>255</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -1897,7 +1915,7 @@
         <v>196</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>202</v>
@@ -1923,12 +1941,17 @@
       <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>247</v>
-      </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" s="4" customFormat="1" ht="216.75" x14ac:dyDescent="0.25">
+      <c r="H9" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>64</v>
       </c>
@@ -1948,11 +1971,12 @@
       <c r="G10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>246</v>
+      <c r="H10" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
@@ -1976,9 +2000,14 @@
         <v>9</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>243</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2004,7 +2033,7 @@
         <v>195</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>202</v>
@@ -2036,7 +2065,7 @@
         <v>199</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>202</v>
@@ -2068,7 +2097,7 @@
         <v>197</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>202</v>
@@ -2218,7 +2247,7 @@
         <v>200</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>202</v>
@@ -2245,10 +2274,10 @@
         <v>8</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>202</v>
@@ -2275,10 +2304,10 @@
         <v>8</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>202</v>
@@ -2308,7 +2337,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="205.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="192.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>106</v>
       </c>
@@ -2332,7 +2361,10 @@
         <v>203</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>238</v>
+        <v>258</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2387,7 +2419,7 @@
         <v>205</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>202</v>
@@ -2436,7 +2468,7 @@
         <v>203</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2461,7 +2493,7 @@
         <v>207</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>202</v>
@@ -2487,7 +2519,7 @@
         <v>207</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>202</v>
@@ -2515,7 +2547,7 @@
         <v>206</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>202</v>
@@ -2543,7 +2575,7 @@
         <v>207</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>202</v>
@@ -2571,7 +2603,7 @@
         <v>203</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2596,7 +2628,7 @@
         <v>208</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>202</v>
@@ -2624,7 +2656,7 @@
         <v>208</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>202</v>
@@ -2652,7 +2684,7 @@
         <v>209</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>202</v>
@@ -2680,7 +2712,7 @@
         <v>203</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2707,7 +2739,7 @@
         <v>210</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>202</v>
@@ -2730,10 +2762,10 @@
         <v>7</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>202</v>
@@ -2787,10 +2819,10 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="14" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>202</v>
@@ -2817,7 +2849,7 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>202</v>
@@ -2928,7 +2960,7 @@
         <v>7</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="J45" s="14" t="s">
         <v>202</v>
@@ -2958,7 +2990,7 @@
         <v>199</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J46" s="14" t="s">
         <v>202</v>
@@ -2986,7 +3018,7 @@
         <v>211</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -3006,7 +3038,7 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I48" s="14" t="s">
         <v>202</v>
@@ -3033,7 +3065,7 @@
         <v>210</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J49" s="14" t="s">
         <v>202</v>
@@ -3057,7 +3089,7 @@
         <v>212</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J50" s="14" t="s">
         <v>202</v>
@@ -3082,7 +3114,7 @@
       <c r="H51" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="I51" s="14" t="s">
+      <c r="I51" s="23" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3102,11 +3134,11 @@
       <c r="G52" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I52" s="14" t="s">
+      <c r="I52" s="23" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
         <v>228</v>
       </c>
@@ -3122,8 +3154,11 @@
       <c r="G53" s="17" t="s">
         <v>9</v>
       </c>
+      <c r="H53" s="23" t="s">
+        <v>231</v>
+      </c>
       <c r="I53" s="14" t="s">
-        <v>231</v>
+        <v>259</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3146,7 +3181,7 @@
         <v>232</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J54" s="14" t="s">
         <v>202</v>
@@ -3171,6 +3206,9 @@
       <c r="H55" s="14" t="s">
         <v>233</v>
       </c>
+      <c r="J55" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="56" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
@@ -3213,34 +3251,45 @@
         <v>234</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J57" s="14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
-        <v>250</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="I58" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="E59" s="23" t="s">
-        <v>252</v>
+        <v>260</v>
+      </c>
+      <c r="I59" s="14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="E60" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="I60" s="14" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G151:G155" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G150:G154" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Priority Names.A1-3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G21 G25:G150" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G21 G25:G149" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>PriorityNames</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Final committee review with all comments resolved
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-First.xlsx
+++ b/MHDS/MHDS-Comment-First.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0445986-88BD-4396-B2FE-45ABA838B625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DADFAAD-F42E-40D7-91C9-44F25040D861}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comment Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="266">
   <si>
     <t>Priority</t>
   </si>
@@ -943,9 +943,6 @@
     <t>research</t>
   </si>
   <si>
-    <t>decided to fully support this option, which means adding an option on MHD for non-contained</t>
-  </si>
-  <si>
     <t>agreed under the option this would be the case</t>
   </si>
   <si>
@@ -1036,9 +1033,6 @@
     <t>add a discussion of organization requirements when they choose to host the binary elswhere</t>
   </si>
   <si>
-    <t>simply close the issue as this is already allowed by MHD… check that assertion</t>
-  </si>
-  <si>
     <t>need to pick a scope pattern, and create an open issue asking for comment on the scope pattern we chose.</t>
   </si>
   <si>
@@ -1052,6 +1046,15 @@
   </si>
   <si>
     <t xml:space="preserve">Lynn is improving them given current discussions. </t>
+  </si>
+  <si>
+    <t>update open issues</t>
+  </si>
+  <si>
+    <t>UnContained option includes</t>
+  </si>
+  <si>
+    <t>decided to fully support this option, which means adding an option on MHD for UnContained</t>
   </si>
 </sst>
 </file>
@@ -1319,13 +1322,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1666,13 +1669,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1721,7 @@
         <v>192</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
@@ -1742,7 +1745,12 @@
       <c r="H2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1798,7 +1806,7 @@
         <v>193</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>202</v>
@@ -1829,8 +1837,11 @@
       <c r="H5" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>264</v>
+      <c r="I5" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1882,10 +1893,10 @@
         <v>8</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>202</v>
@@ -1915,7 +1926,7 @@
         <v>196</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>202</v>
@@ -1942,10 +1953,10 @@
         <v>8</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>202</v>
@@ -1972,7 +1983,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="4" t="s">
@@ -2000,10 +2011,10 @@
         <v>9</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>202</v>
@@ -2033,7 +2044,7 @@
         <v>195</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>202</v>
@@ -2065,7 +2076,7 @@
         <v>199</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>202</v>
@@ -2097,7 +2108,7 @@
         <v>197</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>202</v>
@@ -2247,7 +2258,7 @@
         <v>200</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>202</v>
@@ -2274,10 +2285,10 @@
         <v>8</v>
       </c>
       <c r="H20" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>202</v>
@@ -2304,10 +2315,10 @@
         <v>8</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>202</v>
@@ -2360,8 +2371,8 @@
       <c r="H23" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>258</v>
+      <c r="I23" s="23" t="s">
+        <v>257</v>
       </c>
       <c r="J23" s="14" t="s">
         <v>202</v>
@@ -2419,7 +2430,7 @@
         <v>205</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J25" s="14" t="s">
         <v>202</v>
@@ -2468,7 +2479,7 @@
         <v>203</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -2493,7 +2504,7 @@
         <v>207</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J28" s="14" t="s">
         <v>202</v>
@@ -2519,7 +2530,7 @@
         <v>207</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>202</v>
@@ -2547,7 +2558,7 @@
         <v>206</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J30" s="14" t="s">
         <v>202</v>
@@ -2575,7 +2586,7 @@
         <v>207</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J31" s="14" t="s">
         <v>202</v>
@@ -2603,7 +2614,10 @@
         <v>203</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2628,7 +2642,7 @@
         <v>208</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J33" s="14" t="s">
         <v>202</v>
@@ -2656,7 +2670,7 @@
         <v>208</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J34" s="14" t="s">
         <v>202</v>
@@ -2684,7 +2698,7 @@
         <v>209</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>202</v>
@@ -2712,7 +2726,10 @@
         <v>203</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2739,7 +2756,7 @@
         <v>210</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>202</v>
@@ -2762,10 +2779,10 @@
         <v>7</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>202</v>
@@ -2819,10 +2836,10 @@
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>202</v>
@@ -2849,7 +2866,7 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>202</v>
@@ -2960,7 +2977,7 @@
         <v>7</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J45" s="14" t="s">
         <v>202</v>
@@ -2990,7 +3007,7 @@
         <v>199</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J46" s="14" t="s">
         <v>202</v>
@@ -3018,7 +3035,10 @@
         <v>211</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="240" x14ac:dyDescent="0.25">
@@ -3038,7 +3058,7 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I48" s="14" t="s">
         <v>202</v>
@@ -3065,7 +3085,7 @@
         <v>210</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J49" s="14" t="s">
         <v>202</v>
@@ -3089,7 +3109,7 @@
         <v>212</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J50" s="14" t="s">
         <v>202</v>
@@ -3114,8 +3134,11 @@
       <c r="H51" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="I51" s="23" t="s">
-        <v>230</v>
+      <c r="I51" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="J51" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="51" x14ac:dyDescent="0.25">
@@ -3134,8 +3157,11 @@
       <c r="G52" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="I52" s="23" t="s">
-        <v>231</v>
+      <c r="I52" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="J52" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -3154,11 +3180,14 @@
       <c r="G53" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="23" t="s">
-        <v>231</v>
+      <c r="H53" s="24" t="s">
+        <v>230</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>259</v>
+        <v>264</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3178,10 +3207,10 @@
         <v>9</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J54" s="14" t="s">
         <v>202</v>
@@ -3204,7 +3233,7 @@
         <v>9</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J55" s="14" t="s">
         <v>202</v>
@@ -3227,7 +3256,7 @@
         <v>9</v>
       </c>
       <c r="H56" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J56" s="14" t="s">
         <v>202</v>
@@ -3248,10 +3277,10 @@
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J57" s="14" t="s">
         <v>202</v>
@@ -3259,29 +3288,46 @@
     </row>
     <row r="58" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="22" t="s">
         <v>246</v>
-      </c>
-      <c r="E58" s="23" t="s">
-        <v>247</v>
       </c>
       <c r="I58" s="14" t="s">
         <v>195</v>
       </c>
+      <c r="J58" s="14" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="E59" s="23" t="s">
+      <c r="E59" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="I59" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="J59" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="E60" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="I60" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="I59" s="14" t="s">
+      <c r="J60" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E61" s="14" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="E60" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="I60" s="14" t="s">
-        <v>262</v>
+      <c r="J61" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final committee comments integrated
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-First.xlsx
+++ b/MHDS/MHDS-Comment-First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DADFAAD-F42E-40D7-91C9-44F25040D861}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8626CA-F8B0-4545-8E3B-F12572DC9FA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="290">
   <si>
     <t>Priority</t>
   </si>
@@ -1055,6 +1055,78 @@
   </si>
   <si>
     <t>decided to fully support this option, which means adding an option on MHD for UnContained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">graphic to include CA or not? </t>
+  </si>
+  <si>
+    <t>CA is a critical aspect of bringing an HIE together. IHE didn't need to profile it, but it is critical</t>
+  </si>
+  <si>
+    <t>Spencer LaGesse</t>
+  </si>
+  <si>
+    <t>Move Storage of Binary to after "When the document recipient is triggered"</t>
+  </si>
+  <si>
+    <t>change "Recipient" in WebSequence diagram to "Consumer"</t>
+  </si>
+  <si>
+    <t>remove blue diagrams in section X.6 -- no need for a diagram since they were included above.</t>
+  </si>
+  <si>
+    <t>the STX options would not be used with ARR, right?</t>
+  </si>
+  <si>
+    <t>NO, the ARR needs security too</t>
+  </si>
+  <si>
+    <t>X.7.2.8</t>
+  </si>
+  <si>
+    <t>given MHDS is only centeralized, should we include federated or push</t>
+  </si>
+  <si>
+    <t>NO, because it is true we will likely need to federate eventually. The scope of centeralized is just the current project</t>
+  </si>
+  <si>
+    <t>X.7.3</t>
+  </si>
+  <si>
+    <t>duplicate definitions of direct, centeralized, and federated</t>
+  </si>
+  <si>
+    <t>eliminate duplicate</t>
+  </si>
+  <si>
+    <t>X.7.3.3</t>
+  </si>
+  <si>
+    <t>should we hint at future federation for MHDS?</t>
+  </si>
+  <si>
+    <t>X.7.5</t>
+  </si>
+  <si>
+    <t>mCSD does not support attributes intended directly for Access Control. </t>
+  </si>
+  <si>
+    <t> This seems out of place. Expand or remove?</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>No, too dangerous to predict the future</t>
+  </si>
+  <si>
+    <t>move Document Registry first in .1, followed by bullet on why, followed by Lynn's full document, follwed by explination</t>
+  </si>
+  <si>
+    <t>yes, but remove profile acronyms to make more clear it is abstract. Move up to 1. section</t>
+  </si>
+  <si>
+    <t>Lynn will make diagrams for X.4</t>
   </si>
 </sst>
 </file>
@@ -1669,13 +1741,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J62" sqref="J62"/>
+      <selection pane="bottomRight" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3301,6 +3373,9 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>245</v>
+      </c>
       <c r="E59" s="22" t="s">
         <v>258</v>
       </c>
@@ -3312,6 +3387,9 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>245</v>
+      </c>
       <c r="E60" s="22" t="s">
         <v>259</v>
       </c>
@@ -3323,11 +3401,177 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>245</v>
+      </c>
       <c r="E61" s="14" t="s">
         <v>263</v>
       </c>
       <c r="J61" s="14" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="I62" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="J62" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="J63" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="J64" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="I66" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J66" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J67" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="I68" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="J69" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="H70" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="I72" s="14" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>